<commit_message>
[Modified, Add]: Add more functions and table headings. Add .docx file
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManageUserInfo/ManageUserInfo.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/ManageUserInfo/ManageUserInfo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\projects\To-Do-App\ToDoApp-Doc\Document\Diagram\Thiết kế phần mềm\Thiết kế xử lý\ManageUserInfo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\projects\To-Do-App\ToDoApp-Doc\Document\Diagram\Thiết Kế Phần Mềm\Thiết Kế Xử Lý\ManageUserInfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="123">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -596,6 +596,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -606,9 +609,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -831,8 +831,8 @@
   </sheetPr>
   <dimension ref="A1:AF1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA16" workbookViewId="0">
-      <selection activeCell="AB20" sqref="AB20"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -868,48 +868,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="52.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="18" t="s">
+      <c r="M1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="20"/>
+      <c r="P1" s="20"/>
+      <c r="Q1" s="20"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="18" t="s">
+      <c r="S1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
-      <c r="W1" s="19"/>
-      <c r="X1" s="19"/>
+      <c r="T1" s="20"/>
+      <c r="U1" s="20"/>
+      <c r="V1" s="20"/>
+      <c r="W1" s="20"/>
+      <c r="X1" s="20"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="18" t="s">
+      <c r="Z1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="AA1" s="19"/>
-      <c r="AB1" s="19"/>
-      <c r="AC1" s="19"/>
-      <c r="AD1" s="19"/>
-      <c r="AE1" s="19"/>
-      <c r="AF1" s="19"/>
+      <c r="AA1" s="20"/>
+      <c r="AB1" s="20"/>
+      <c r="AC1" s="20"/>
+      <c r="AD1" s="20"/>
+      <c r="AE1" s="20"/>
+      <c r="AF1" s="20"/>
     </row>
     <row r="2" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -1056,10 +1056,10 @@
       <c r="V3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="W3" s="20" t="s">
+      <c r="W3" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="X3" s="23" t="s">
+      <c r="X3" s="24" t="s">
         <v>28</v>
       </c>
       <c r="Y3" s="1"/>
@@ -1130,8 +1130,8 @@
       <c r="V4" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="W4" s="21"/>
-      <c r="X4" s="21"/>
+      <c r="W4" s="22"/>
+      <c r="X4" s="22"/>
       <c r="Y4" s="9"/>
       <c r="Z4" s="6">
         <v>2</v>
@@ -1163,14 +1163,14 @@
       <c r="C5" s="5"/>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
       <c r="L5" s="1"/>
       <c r="M5" s="10">
         <v>3</v>
@@ -1198,8 +1198,8 @@
       <c r="V5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="W5" s="21"/>
-      <c r="X5" s="21"/>
+      <c r="W5" s="22"/>
+      <c r="X5" s="22"/>
       <c r="Y5" s="9"/>
       <c r="Z5" s="6">
         <v>3</v>
@@ -1231,23 +1231,23 @@
       <c r="C6" s="5"/>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="5">
-        <v>1</v>
+      <c r="F6" s="3" t="s">
+        <v>5</v>
       </c>
-      <c r="G6" s="5" t="s">
-        <v>36</v>
+      <c r="G6" s="3" t="s">
+        <v>9</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>34</v>
+      <c r="H6" s="3" t="s">
+        <v>10</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>38</v>
+      <c r="I6" s="3" t="s">
+        <v>11</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>52</v>
+      <c r="J6" s="3" t="s">
+        <v>12</v>
       </c>
-      <c r="K6" s="5" t="s">
-        <v>53</v>
+      <c r="K6" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="L6" s="1"/>
       <c r="M6" s="10">
@@ -1276,8 +1276,8 @@
       <c r="V6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="W6" s="21"/>
-      <c r="X6" s="21"/>
+      <c r="W6" s="22"/>
+      <c r="X6" s="22"/>
       <c r="Y6" s="9"/>
       <c r="Z6" s="6">
         <v>4</v>
@@ -1309,22 +1309,24 @@
       <c r="C7" s="5"/>
       <c r="D7" s="4"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="10">
-        <v>2</v>
+      <c r="F7" s="5">
+        <v>1</v>
       </c>
-      <c r="G7" s="10" t="s">
-        <v>45</v>
+      <c r="G7" s="5" t="s">
+        <v>36</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="I7" s="10" t="s">
-        <v>62</v>
+      <c r="I7" s="5" t="s">
+        <v>38</v>
       </c>
-      <c r="J7" s="10" t="s">
-        <v>63</v>
+      <c r="J7" s="5" t="s">
+        <v>52</v>
       </c>
-      <c r="K7" s="10"/>
+      <c r="K7" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="L7" s="1"/>
       <c r="M7" s="10">
         <v>5</v>
@@ -1352,8 +1354,8 @@
       <c r="V7" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
+      <c r="W7" s="22"/>
+      <c r="X7" s="22"/>
       <c r="Y7" s="1"/>
       <c r="Z7" s="5">
         <v>5</v>
@@ -1386,21 +1388,21 @@
       <c r="D8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H8" s="10" t="s">
         <v>34</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="J8" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K8" s="11"/>
+      <c r="K8" s="10"/>
       <c r="L8" s="1"/>
       <c r="M8" s="10">
         <v>6</v>
@@ -1428,8 +1430,8 @@
       <c r="V8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="22"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
       <c r="Y8" s="13"/>
       <c r="Z8" s="5">
         <v>6</v>
@@ -1466,16 +1468,16 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="H9" s="10" t="s">
         <v>34</v>
       </c>
       <c r="I9" s="10" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="J9" s="10" t="s">
         <v>63</v>
@@ -1534,16 +1536,16 @@
       <c r="D10" s="4"/>
       <c r="E10" s="1"/>
       <c r="F10" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="H10" s="10" t="s">
         <v>34</v>
       </c>
       <c r="I10" s="10" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J10" s="10" t="s">
         <v>63</v>
@@ -1601,22 +1603,22 @@
       <c r="C11" s="5"/>
       <c r="D11" s="4"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="5">
-        <v>6</v>
+      <c r="F11" s="10">
+        <v>5</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>82</v>
+      <c r="G11" s="10" t="s">
+        <v>72</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="I11" s="5" t="s">
-        <v>93</v>
+      <c r="I11" s="10" t="s">
+        <v>87</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="K11" s="5"/>
+      <c r="K11" s="11"/>
       <c r="L11" s="1"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
@@ -1666,16 +1668,16 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="5">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="H12" s="5" t="s">
         <v>34</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="J12" s="5" t="s">
         <v>63</v>
@@ -1721,12 +1723,22 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="F13" s="5">
+        <v>7</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="K13" s="5"/>
       <c r="L13" s="1"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
@@ -2073,7 +2085,7 @@
       <c r="AA20" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="AB20" s="24" t="s">
+      <c r="AB20" s="18" t="s">
         <v>121</v>
       </c>
       <c r="AC20" s="10" t="s">
@@ -35444,6 +35456,7 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="Z1:AF1"/>
     <mergeCell ref="F5:K5"/>
     <mergeCell ref="W3:W8"/>
     <mergeCell ref="X3:X8"/>
@@ -35451,7 +35464,6 @@
     <mergeCell ref="F1:K1"/>
     <mergeCell ref="M1:Q1"/>
     <mergeCell ref="S1:X1"/>
-    <mergeCell ref="Z1:AF1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>